<commit_message>
update selected function for auto testing
</commit_message>
<xml_diff>
--- a/Auto_TC.xlsx
+++ b/Auto_TC.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="LOGIN" sheetId="1" r:id="rId1"/>
     <sheet name="REGISTER" sheetId="2" r:id="rId2"/>
     <sheet name="FORGOT_PASSWORD" sheetId="3" r:id="rId3"/>
-    <sheet name="COLLECTION" sheetId="4" r:id="rId4"/>
+    <sheet name="PUBLISHER" sheetId="4" r:id="rId4"/>
     <sheet name="ACCOUNT" sheetId="5" r:id="rId5"/>
     <sheet name="Overview" sheetId="6" r:id="rId6"/>
   </sheets>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="243">
   <si>
     <t>TEST CASES</t>
   </si>
@@ -595,346 +595,6 @@
   <si>
     <t>7. Hiển thị icon cảnh báo, với tiêu đề thông báo "cảnh báo", nội dung: "Chưa có tài khoản đăng kí trong hệ thống"
 8. Tắt thông báo</t>
-  </si>
-  <si>
-    <t>COLLECTION_F_02</t>
-  </si>
-  <si>
-    <t>Thêm thông tin bộ truyện với tên bộ truyện có 1 kí tự và có chọn tác giả, nhà xuất bản, ngày phát hành, tình trạng</t>
-  </si>
-  <si>
-    <t>Đã đăng nhập thành công và đã lưu trữ ít nhất hai thông tin về tác giả và nhà xuất bản</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B1: Tại giao diện trang chủ, chọn nút bộ truyện hoặc chọn mục bộ truyện trong menu
-B2: Chọn nút "+" để mở giao diện thông tin bộ truyện
-B3: Chọn trường tên bộ truyện và nhập: 's'
-B4: Chọn dropdown tác giả và chọn vị trí thứ 2
-B5:  Chọn dropdown nhà xuất bản và chọn vị trí thứ 2
-B6:  Chọn dropdown tình trạng và chọn vị trí thứ 2
-B7:   Chọn ngày phát hành và chọn ngày trước ngày hiện tại
-B8: Chọn nút "+" để thêm thông tin
-B9: Chọn nút "Ok" trên thông báo
-</t>
-  </si>
-  <si>
-    <t>2. Hiển thị giao diện thông tin bộ truyện với mã bộ truyện đã được tạo sẵn
-8. Hiển thị với icon thành công, tiêu đề: "Thông báo" và nội dung: "Thêm thông tin bộ truyện thành công" 
-9. Tắt thông báo và làm mới các trường nhập đồng thời tạo mới mã bộ truyện</t>
-  </si>
-  <si>
-    <t>COLLECTION_F_03</t>
-  </si>
-  <si>
-    <t>Thêm thông tin bộ truyện với tên bộ truyện có 2 kí tự và có chọn tác giả, nhà xuất bản, ngày phát hành, tình trạng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B1: Tại giao diện trang chủ, chọn nút bộ truyện hoặc chọn mục bộ truyện trong menu
-B2: Chọn nút "+" để mở giao diện thông tin bộ truyện
-B3: Chọn trường tên bộ truyện và nhập: 'sp'
-B4: Chọn dropdown tác giả và chọn vị trí thứ 2
-B5:  Chọn dropdown nhà xuất bản và chọn vị trí thứ 2
-B6:  Chọn dropdown tình trạng và chọn vị trí thứ 2
-B7:   Chọn ngày phát hành và chọn ngày trước ngày hiện tại
-B8: Chọn nút "+" để thêm thông tin
-B9: Chọn nút "Ok" trên thông báo
-</t>
-  </si>
-  <si>
-    <t>COLLECTION_F_04</t>
-  </si>
-  <si>
-    <t>Thêm thông tin bộ truyện với tên bộ truyện có 2 kí tự và có chọn tác giả, nhà xuất bản, ngày phát hành, tình trạng và ghi chú có 1 kí tự</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B1: Tại giao diện trang chủ, chọn nút bộ truyện hoặc chọn mục bộ truyện trong menu
-B2: Chọn nút "+" để mở giao diện thông tin bộ truyện
-B3: Chọn trường tên bộ truyện và nhập: 'sp'
-B4: Chọn dropdown tác giả và chọn vị trí thứ 2
-B5:  Chọn dropdown nhà xuất bản và chọn vị trí thứ 2
-B6:  Chọn dropdown tình trạng và chọn vị trí thứ 2
-B7:   Chọn ngày phát hành và chọn ngày trước ngày hiện tại
-B8:  Chọn trường ghi chú và nhập: 'g'
-B9: Chọn nút "+" để thêm thông tin
-B10: Chọn nút "Ok" trên thông báo
-</t>
-  </si>
-  <si>
-    <t>2. Hiển thị giao diện thông tin bộ truyện với mã bộ truyện đã được tạo sẵn
-5. Hiển thị với icon thành công, tiêu đề: "Thông báo" và nội dung: "Thêm thông tin bộ truyện thành công" 
-6. Tắt thông báo và làm mới các trường nhập đồng thời tạo mới mã bộ truyện</t>
-  </si>
-  <si>
-    <t>COLLECTION_F_05</t>
-  </si>
-  <si>
-    <t>Thêm thông tin bộ truyện với tên bộ truyện có 2 kí tự và không chọn tác giả, nhà xuất bản, ngày phát hành, tình trạng và ghi chú có 1 kí tự</t>
-  </si>
-  <si>
-    <t>Đã đăng nhập thành công và đã lưu trữ ít nhất một thông tin về tác giả và nhà xuất bản</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B1: Tại giao diện trang chủ, chọn nút bộ truyện hoặc chọn mục bộ truyện trong menu
-B2: Chọn nút "+" để mở giao diện thông tin bộ truyện
-B3: Chọn trường tên bộ truyện và nhập: 'sp'
-B4:  Chọn trường ghi chú và nhập: 'g'
-B5: Chọn nút "+" để thêm thông tin
-B6: Chọn nút "Ok" trên thông báo
-</t>
-  </si>
-  <si>
-    <t>2. Hiển thị giao diện thông tin bộ truyện với mã bộ truyện đã được tạo sẵn
-9. Hiển thị với icon thành công, tiêu đề: "Thông báo" và nội dung: "Thêm thông tin bộ truyện thành công" 
-10. Tắt thông báo và làm mới các trường nhập đồng thời tạo mới mã bộ truyện</t>
-  </si>
-  <si>
-    <t>COLLECTION_F_06</t>
-  </si>
-  <si>
-    <t>Thêm thông tin bộ truyện với trường tên bộ truyện bị bỏ trống</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B1: Tại giao diện trang chủ, chọn nút bộ truyện hoặc chọn mục bộ truyện trong menu
-B2: Chọn nút "+" để mở giao diện thông tin bộ truyện
-B3:  Chọn trường ghi chú và nhập: 'g'
-B4: Chọn nút "+" để thêm thông tin
-B5: Chọn nút "Ok" trên thông báo
-</t>
-  </si>
-  <si>
-    <t>2. Hiển thị giao diện thông tin bộ truyện với mã bộ truyện đã được tạo sẵn
-4. Hiển thị icon cảnh báo, với tiêu đề thông báo "Cảnh báo", nội dung: "Không được bỏ trống tên bộ truyện"
-5. Tắt thông báo</t>
-  </si>
-  <si>
-    <t>COLLECTION_F_07</t>
-  </si>
-  <si>
-    <t>Thêm thông tin bộ truyện với chưa có thông tin tác giả và nhà xuất bản được lưu</t>
-  </si>
-  <si>
-    <t>Đã đăng nhập thành công và chưa lưu thông tin tác giả và nhà xuất bản nào</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B1: Tại giao diện trang chủ, chọn nút bộ truyện hoặc chọn mục bộ truyện trong menu
-B2: Chọn nút "+" để mở giao diện thông tin bộ truyện
-B3:  Chọn tên bộ truyện và nhập: 'spyxfamily'
-B4: Chọn nút "+" để thêm thông tin
-B5: Chọn nút "Ok" trên thông báo
-</t>
-  </si>
-  <si>
-    <t>2. Hiển thị giao diện thông tin bộ truyện với mã bộ truyện đã được tạo sẵn
-4. Hiển thị icon thất bại, với tiêu đề thông báo "Thông báo", nội dung: "Thêm bộ truyện không thành công"
-5. Tắt thông báo</t>
-  </si>
-  <si>
-    <t>COLLECTION_F_08</t>
-  </si>
-  <si>
-    <t>Thêm thông tin bộ truyện đã tồn tại</t>
-  </si>
-  <si>
-    <t>Đã đăng nhập thành công
-Có ít nhất một thông tin bộ truyện đã được lưu trong danh sách</t>
-  </si>
-  <si>
-    <t>B1: Tại giao diện trang chủ, chọn nút bộ truyện hoặc chọn mục bộ truyện trong menu
-B2: Trong danh sách thông tin bộ truyện, chọn vào thông tin đầu tiền
-B3: Chọn "+" để thêm thông tin bộ truyện
-B4: Chọn nút "OK" trong thông báo</t>
-  </si>
-  <si>
-    <t>2. Hiển thị thông tin bộ truyện được chọn trên các trường tương ứng
-3. Hiển thị icon thất bại, tiêu đề: "Thông báo" và nội dung: "Thêm thông tin bộ truyện không thành công"
-4. Tắt thông báo</t>
-  </si>
-  <si>
-    <t>COLLECTION_F_09</t>
-  </si>
-  <si>
-    <t>Sửa thông tin bộ truyện với tên bộ truyện có 2 kí tự, thay đổi tác giả, nhà xuất bản, tình trạng và ngày phát hành</t>
-  </si>
-  <si>
-    <t>Đã đăng nhập thành công
-Có ít nhất một thông tin bộ truyện đã được lưu trong danh sách
-Có ít nhất 2 thông tin trong tác giả và nhà xuất bản được lưu trong hệ thống</t>
-  </si>
-  <si>
-    <t>B1: Tại giao diện trang chủ, chọn nút bộ truyện hoặc chọn mục bộ truyện trong menu
-B2: Trong danh sách thông tin bộ truyện, chọn vào thông tin đầu tiên
-B3: Chọn trường tên bộ truyện, xóa thông tin cũ và nhập: 'hi'
-B4: Chọn dropdown tác giả và chọn vị trí thứ 2
-B5:  Chọn dropdown nhà xuất bản và chọn vị trí thứ 2
-B6:  Chọn dropdown tình trạng và chọn vị trí thứ 2
-B7:   Chọn ngày phát hành và chọn ngày trước ngày hiện tại
-B8: Chọn sửa để sửa thông tin bộ truyện
-B9: Chọn nút "OK" trong thông báo</t>
-  </si>
-  <si>
-    <t>2. Hiển thị thông tin bộ truyện được chọn trên các trường tương ứng
-8. Hiển thị icon thành công, với tiêu đề thông báo "Thông báo", nội dung: "Sửa thông tin bộ truyện thành công"
-9. Tắt thông báo và trở về danh sách thông tin bộ truyện</t>
-  </si>
-  <si>
-    <t>COLLECTION_F_10</t>
-  </si>
-  <si>
-    <t>Sửa thông tin bộ truyện với tên bộ truyện có 1 kí tự và ghi chú có 1 kí tự</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Đã đăng nhập thành công
-Có ít nhất một thông tin bộ truyện đã được lưu trong danh sách
-</t>
-  </si>
-  <si>
-    <t>B1: Tại giao diện trang chủ, chọn nút bộ truyện hoặc chọn mục bộ truyện trong menu
-B2: Trong danh sách thông tin bộ truyện, chọn vào thông tin đầu tiên
-B3: Chọn trường tên bộ truyện, xóa thông tin cũ và nhập: 'h'
-B4: Chọn trường ghi chú và nhập: 'g'
-B5: Chọn sửa để sửa thông tin bộ truyện
-B6: Chọn nút "OK" trong thông báo</t>
-  </si>
-  <si>
-    <t>2. Hiển thị thông tin bộ truyện được chọn trên các trường tương ứng
-5. Hiển thị icon thành công, với tiêu đề thông báo "Thông báo", nội dung: "Sửa thông tin bộ truyện thành công"
-6. Tắt thông báo và trở về danh sách thông tin bộ truyện</t>
-  </si>
-  <si>
-    <t>COLLECTION_F_11</t>
-  </si>
-  <si>
-    <t>Sửa thông tin bộ truyện với tên bộ truyện bị bỏ trống</t>
-  </si>
-  <si>
-    <t>B1: Tại giao diện trang chủ, chọn nút bộ truyện hoặc chọn mục bộ truyện trong menu
-B2: Trong danh sách thông tin bộ truyện, chọn vào thông tin đầu tiên
-B3: Chọn trường tên bộ truyện, xóa thông tin cũ 
-B4: Chọn sửa để sửa thông tin bộ truyện
-B5: Chọn nút "OK" trong thông báo</t>
-  </si>
-  <si>
-    <t>2. Hiển thị thông tin bộ truyện được chọn trên các trường tương ứng
-4. Hiển thị icon cảnh báo, với tiêu đề thông báo "Cảnh báo", nội dung: "Không được bỏ trống tên bộ truyện"
-5. Tắt thông báo</t>
-  </si>
-  <si>
-    <t>COLLECTION_F_12</t>
-  </si>
-  <si>
-    <t>Sửa thông tin bộ truyện không tồn tại</t>
-  </si>
-  <si>
-    <t>B1: Tại giao diện trang chủ, chọn nút bộ truyện hoặc chọn mục bộ truyện trong menu
-B2: Chọn nút "+" để mở giao diện thông tin bộ truyện
-B3: Chọn sửa thông tin bộ truyện
-B4: Nhấn "OK" trên thông báo</t>
-  </si>
-  <si>
-    <t>2. Hiển thị giao diện thông tin bộ truyện với mã bộ truyện đã được tạo sẵn
-3. Hiển thị icon thất bại, với tiêu đề thông báo "Thông báo", nội dung: "Sửa thông tin bộ truyện không thành công"
-4. Tắt thông báo</t>
-  </si>
-  <si>
-    <t>COLLECTION_F_13</t>
-  </si>
-  <si>
-    <t>Xóa thông tin bộ truyện thành công</t>
-  </si>
-  <si>
-    <t>B1: Tại giao diện trang chủ, chọn nút bộ truyện hoặc chọn mục bộ truyện trong menu
-B2: Trong danh sách thông tin bộ truyện, chọn vào thông tin đầu tiên
-B3: Chọn nút xóa
-B4: Chọn nút "OK" trong thông báo</t>
-  </si>
-  <si>
-    <t>2. Hiển thị thông tin bộ truyện được chọn trên các trường tương ứng
-3. Hiển thị icon thông báo, với tiêu đề thông báo "Thông báo", nội dung: "Bạn có chắc chắn muốn xóa thông tin này không"
-4. Tắt thông báo và trở lại danh sách thông tin bộ truyện</t>
-  </si>
-  <si>
-    <t>COLLECTION_F_14</t>
-  </si>
-  <si>
-    <t>Không xóa thông tin bộ truyện</t>
-  </si>
-  <si>
-    <t>B1: Tại giao diện trang chủ, chọn nút bộ truyện hoặc chọn mục bộ truyện trong menu
-B2: Trong danh sách thông tin bộ truyện, chọn vào thông tin đầu tiên
-B3: Chọn nút xóa
-B4: Chọn nút "CANCEL" trong thông báo</t>
-  </si>
-  <si>
-    <t>2. Hiển thị thông tin bộ truyện được chọn trên các trường tương ứng
-3. Hiển thị icon thông báo, với tiêu đề thông báo "Thông báo", nội dung: "Bạn có chắc chắn muốn xóa thông tin này không"
-4. Tắt thông báo</t>
-  </si>
-  <si>
-    <t>COLLECTION_F_15</t>
-  </si>
-  <si>
-    <t>Xóa thông tin bộ truyện không tồn tại</t>
-  </si>
-  <si>
-    <t>B1: Tại giao diện trang chủ, chọn nút bộ truyện hoặc chọn mục bộ truyện trong menu
-B2: Chọn nút "+" để mở giao diện thông tin bộ truyện
-B3: Chọn nút xóa
-B4: Chọn nút "OK" trong thông báo
-B5: Chọn nút "OK" trong thông báo</t>
-  </si>
-  <si>
-    <t>2. Hiển thị thông tin bộ truyện được chọn trên các trường tương ứng
-3. Hiển thị icon thông báo, với tiêu đề thông báo "Thông báo", nội dung: "Bạn có chắc chắn muốn xóa thông tin này không"
-4. Hiển thị icon thông báo, với tiêu đề thông báo "Thông báo", nội dung: "Xóa thông tin bộ truyện không thành công"</t>
-  </si>
-  <si>
-    <t>COLLECTION_F_16</t>
-  </si>
-  <si>
-    <t>Tìm kiếm thông tin bộ truyện với tên bộ truyện tồn tại</t>
-  </si>
-  <si>
-    <t>Đã đăng nhập thành công
-Có ít nhất một thông tin bộ truyện đã được lưu trong danh sách với tên 'spyxfamily'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B1: Tại giao diện trang chủ, chọn nút bộ truyện hoặc chọn mục bộ truyện trong menu
-B2: Chọn nút tìm kiếm
-B3: Chọn ô tìm kiếm và nhập: 'spyxfamily'
-</t>
-  </si>
-  <si>
-    <t>3. Hiển thị thông tin các bộ truyện có tên 'spyxfamily'</t>
-  </si>
-  <si>
-    <t>COLLECTION_F_17</t>
-  </si>
-  <si>
-    <t>Tìm kiếm thông tin bộ truyện với tên bộ truyện bị bỏ trống</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B1: Tại giao diện trang chủ, chọn nút bộ truyện hoặc chọn mục bộ truyện trong menu
-B2: Chọn nút tìm kiếm
-B3: Chọn ô tìm kiếm và nhập: 'spyxfamily'
-B4: Xóa thông tin trong ô tìm kiếm
-</t>
-  </si>
-  <si>
-    <t>3. Hiển thị thông tin các bộ truyện có tên 'spyxfamily'
-4. Hiển thị toàn bộ thông tin các bộ truyện đã được lưu trữ</t>
-  </si>
-  <si>
-    <t>COLLECTION_F_18</t>
-  </si>
-  <si>
-    <t>Tìm kiếm thông tin bộ truyện với tên bộ truyện không tồn tại</t>
-  </si>
-  <si>
-    <t>Đã đăng nhập thành công
-Có ít nhất một thông tin bộ truyện đã được lưu trong danh sách và không có bộ truyện nào có tên "spyxfamily"</t>
-  </si>
-  <si>
-    <t>3. Không hiển thị thông tin bộ truyện nào trong danh sách</t>
   </si>
   <si>
     <t>SETUP_ACCOUNT_F_00</t>
@@ -1120,9 +780,6 @@
     <t>Quên mật khẩu</t>
   </si>
   <si>
-    <t>Quản lý thông tin bộ truyện</t>
-  </si>
-  <si>
     <t>Thiết lập tài khoản</t>
   </si>
   <si>
@@ -1133,6 +790,334 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>PUBLISHER_F_02</t>
+  </si>
+  <si>
+    <t>Thêm thông tin nhà xuất bản với tên nhà xuất bản có 1 kí tự và số điện thoại hợp lệ</t>
+  </si>
+  <si>
+    <t>Đã đăng nhập thành công</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1: Tại giao diện trang chủ, chọn nút nhà xuất bản hoặc chọn mục nhà xuất bản trong menu
+B2: Chọn nút "+" để mở giao diện thông tin nhà xuất bản
+B3: Chọn trường tên nhà xuất bản và nhập: 'h'
+B4: Chọn trường số điện thoại và nhập: '0123456789'
+B5: Chọn nút "+" để thêm thông tin
+B6: Chọn nút "Ok" trên thông báo
+</t>
+  </si>
+  <si>
+    <t>2. Hiển thị giao diện thông tin nhà xuất bản với mã nhà xuất bản đã được tạo sẵn
+5. Hiển thị với icon thành công, tiêu đề: "Thông báo" và nội dung: "Thêm thông tin nhà xuất bản thành công" 
+6. Tắt thông báo và làm mới các trường nhập đồng thời tạo mới mã nhà xuất bản</t>
+  </si>
+  <si>
+    <t>PUBLISHER_F_03</t>
+  </si>
+  <si>
+    <t>Thêm thông tin nhà xuất bản với tên nhà xuất bản có 2 kí tự và số điện thoại hợp lệ, chọn tình trạng "Tạm dừng"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1: Tại giao diện trang chủ, chọn nút nhà xuất bản hoặc chọn mục nhà xuất bản trong menu
+B2: Chọn nút "+" để mở giao diện thông tin nhà xuất bản
+B3: Chọn trường tên nhà xuất bản và nhập: 'hi'
+B4: Nhấn vào dropbox và chọn "Tạm dừng"
+B5: Chọn trường số điện thoại và nhập: '0123456789'
+B6: Chọn nút "+" để thêm thông tin
+B7: Chọn nút "Ok" trên thông báo
+</t>
+  </si>
+  <si>
+    <t>2. Hiển thị giao diện thông tin nhà xuất bản với mã nhà xuất bản đã được tạo sẵn
+6. Hiển thị với icon thành công, tiêu đề: "Thông báo" và nội dung: "Thêm thông tin nhà xuất bản thành công" 
+7. Tắt thông báo và làm mới các trường nhập đồng thời tạo mới mã nhà xuất bản</t>
+  </si>
+  <si>
+    <t>PUBLISHER_F_04</t>
+  </si>
+  <si>
+    <t>Thêm thông tin nhà xuất bản với tên nhà xuất bản có 2 kí tự, địa chỉ và ghi chú có 1 kí tự và số điện thoại hợp lệ, chọn tình trạng "Không họat động"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1: Tại giao diện trang chủ, chọn nút nhà xuất bản hoặc chọn mục nhà xuất bản trong menu
+B2: Chọn nút "+" để mở giao diện thông tin nhà xuất bản
+B3: Chọn trường tên nhà xuất bản và nhập: 'hi'
+B4: Nhấn vào dropbox và chọn "Không hoạt động"
+B5: Chọn trường số điện thoại và nhập: '0123456789'
+B6: Chọn trường địa chỉ và nhập: 'h'
+B7: Chọn trường ghi chú và nhập: 'h'
+B8: Chọn nút "+" để thêm thông tin
+B9: Chọn nút "Ok" trên thông báo
+</t>
+  </si>
+  <si>
+    <t>2. Hiển thị giao diện thông tin nhà xuất bản với mã nhà xuất bản đã được tạo sẵn
+8. Hiển thị với icon thành công, tiêu đề: "Thông báo" và nội dung: "Thêm thông tin nhà xuất bản thành công" 
+9. Tắt thông báo và làm mới các trường nhập đồng thời tạo mới mã nhà xuất bản</t>
+  </si>
+  <si>
+    <t>PUBLISHER_F_05</t>
+  </si>
+  <si>
+    <t>Thêm thông tin nhà xuất bản với trường tên nhà xuất bản bị bỏ trống</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1: Tại giao diện trang chủ, chọn nút nhà xuất bản hoặc chọn mục nhà xuất bản trong menu
+B2: Chọn nút "+" để mở giao diện thông tin nhà xuất bản
+B3: Chọn trường số điện thoại và nhập: '0123456789'
+B4: Chọn nút "+" để thêm thông tin
+B5: Chọn nút "Ok" trên thông báo
+</t>
+  </si>
+  <si>
+    <t>2. Hiển thị giao diện thông tin nhà xuất bản với mã nhà xuất bản đã được tạo sẵn
+4. Hiển thị icon cảnh báo, với tiêu đề thông báo "Cảnh báo", nội dung: "Không được bỏ trống tên nhà xuất bản"
+5. Tắt thông báo</t>
+  </si>
+  <si>
+    <t>PUBLISHER_F_06</t>
+  </si>
+  <si>
+    <t>Thêm thông tin nhà xuất bản với số điện thoại không hợp lệ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1: Tại giao diện trang chủ, chọn nút nhà xuất bản hoặc chọn mục nhà xuất bản trong menu
+B2: Chọn nút "+" để mở giao diện thông tin nhà xuất bản
+B3: Chọn trường số điện thoại và nhập: '^^&amp;&amp;**789'
+B4: Chọn nút "+" để thêm thông tin
+B5: Chọn nút "Ok" trên thông báo
+</t>
+  </si>
+  <si>
+    <t>2. Hiển thị giao diện thông tin nhà xuất bản với mã nhà xuất bản đã được tạo sẵn
+4. Hiển thị icon cảnh báo, với tiêu đề thông báo "Cảnh báo", nội dung: "Số điện thoại không hợp lệ"
+5. Tắt thông báo</t>
+  </si>
+  <si>
+    <t>PUBLISHER_F_07</t>
+  </si>
+  <si>
+    <t>Thêm thông tin nhà xuất bản đã tồn tại</t>
+  </si>
+  <si>
+    <t>Đã đăng nhập thành công
+Có ít nhất một thông tin nhà xuất bản đã được lưu trong danh sách</t>
+  </si>
+  <si>
+    <t>B1: Tại giao diện trang chủ, chọn nút nhà xuất bản hoặc chọn mục nhà xuất bản trong menu
+B2: Trong danh sách thông tin nhà xuất bản, chọn vào thông tin đầu tiền
+B3: Chọn "+" để thêm thông tin nhà xuất bản
+B4: Chọn nút "OK" trong thông báo</t>
+  </si>
+  <si>
+    <t>2. Hiển thị thông tin nhà xuất bản được chọn trên các trường tương ứng
+3. Hiển thị icon thất bại, tiêu đề: "Thông báo" và nội dung: "Thêm thông tin nhà xuất bản không thành công"
+4. Tắt thông báo</t>
+  </si>
+  <si>
+    <t>PUBLISHER_F_08</t>
+  </si>
+  <si>
+    <t>Sửa thông tin nhà xuất bản với tên nhà xuất bản có 2 kí tự, đổi tình trạng và số điện thoại hợp lệ</t>
+  </si>
+  <si>
+    <t>B1: Tại giao diện trang chủ, chọn nút nhà xuất bản hoặc chọn mục nhà xuất bản trong menu
+B2: Trong danh sách thông tin nhà xuất bản, chọn vào thông tin đầu tiên
+B3: Chọn trường tên nhà xuất bản, xóa thông tin cũ và nhập: 'hi'
+B4: Chọn dropbox và chọn "Tạm dừng"
+B5: Chọn trường số điện thoại, xóa thông tin cũ và nhập: '0123456789'
+B6: Chọn sửa để sửa thông tin nhà xuất bản
+B7: Chọn nút "OK" trong thông báo</t>
+  </si>
+  <si>
+    <t>2. Hiển thị thông tin nhà xuất bản được chọn trên các trường tương ứng
+6. Hiển thị icon thành công, với tiêu đề thông báo "Thông báo", nội dung: "Sửa thông tin nhà xuất bản thành công"
+7. Tắt thông báo và trở về danh sách thông tin nhà xuất bản</t>
+  </si>
+  <si>
+    <t>PUBLISHER_F_09</t>
+  </si>
+  <si>
+    <t>Sửa thông tin nhà xuất bản với tên nhà xuất bản có 1 kí tự, đổi tình trạng và số điện thoại hợp lệ, ghi chú có 1 kí tự</t>
+  </si>
+  <si>
+    <t>B1: Tại giao diện trang chủ, chọn nút nhà xuất bản hoặc chọn mục nhà xuất bản trong menu
+B2: Trong danh sách thông tin nhà xuất bản, chọn vào thông tin đầu tiên
+B3: Chọn trường tên nhà xuất bản, xóa thông tin cũ và nhập: 'h'
+B4: Chọn dropbox và chọn "Tạm dừng"
+B5: Chọn trường số điện thoại, xóa thông tin cũ và nhập: '0123456789'
+B6: Chọn trường ghi chú, xóa thông tin cũ và nhập: "h"
+B7: Chọn sửa để sửa thông tin nhà xuất bản
+B8: Chọn nút "OK" trong thông báo</t>
+  </si>
+  <si>
+    <t>2. Hiển thị thông tin nhà xuất bản được chọn trên các trường tương ứng
+7. Hiển thị icon thành công, với tiêu đề thông báo "Thông báo", nội dung: "Sửa thông tin nhà xuất bản thành công"
+8. Tắt thông báo và trở về danh sách thông tin nhà xuất bản</t>
+  </si>
+  <si>
+    <t>PUBLISHER_F_10</t>
+  </si>
+  <si>
+    <t>Sửa thông tin nhà xuất bản với tên nhà xuất bản bị bỏ trống</t>
+  </si>
+  <si>
+    <t>B1: Tại giao diện trang chủ, chọn nút nhà xuất bản hoặc chọn mục nhà xuất bản trong menu
+B2: Trong danh sách thông tin nhà xuất bản, chọn vào thông tin đầu tiên
+B3: Chọn trường tên nhà xuất bản, xóa thông tin cũ
+B4: Chọn dropbox và chọn "Tạm dừng"
+B5: Chọn trường số điện thoại, xóa thông tin cũ và nhập: '0123456789'
+B6: Chọn sửa để sửa thông tin nhà xuất bản
+B7: Chọn nút "OK" trong thông báo</t>
+  </si>
+  <si>
+    <t>2. Hiển thị thông tin nhà xuất bản được chọn trên các trường tương ứng
+6. Hiển thị icon cảnh báo, với tiêu đề thông báo "Cảnh báo", nội dung: "Không thể bỏ trống tên nhà xuất bản"
+7. Tắt thông báo</t>
+  </si>
+  <si>
+    <t>PUBLISHER_F_11</t>
+  </si>
+  <si>
+    <t>Sửa thông tin nhà xuất bản với số điện thoại không hợp lệ</t>
+  </si>
+  <si>
+    <t>B1: Tại giao diện trang chủ, chọn nút nhà xuất bản hoặc chọn mục nhà xuất bản trong menu
+B2: Trong danh sách thông tin nhà xuất bản, chọn vào thông tin đầu tiên
+B3: Chọn trường tên nhà xuất bản, xóa thông tin cũ và nhập: 'hi'
+B4: Chọn dropbox và chọn "Tạm dừng"
+B5: Chọn trường số điện thoại, xóa thông tin cũ và nhập: '0^&amp;*  123456789'
+B6: Chọn sửa để sửa thông tin nhà xuất bản
+B7: Chọn nút "OK" trong thông báo</t>
+  </si>
+  <si>
+    <t>2. Hiển thị thông tin nhà xuất bản được chọn trên các trường tương ứng
+6. Hiển thị icon cảnh báo, với tiêu đề thông báo "Cảnh báo", nội dung: "Số điện thoại không hợp lệ"
+7. Tắt thông báo</t>
+  </si>
+  <si>
+    <t>PUBLISHER_F_12</t>
+  </si>
+  <si>
+    <t>Sửa thông tin nhà xuất bản không tồn tại</t>
+  </si>
+  <si>
+    <t>B1: Tại giao diện trang chủ, chọn nút nhà xuất bản hoặc chọn mục nhà xuất bản trong menu
+B2: Chọn nút "+" để mở giao diện thông tin nhà xuất bản
+B3: Chọn sửa thông tin nhà xuất bản
+B4: Nhấn "OK" trên thông báo</t>
+  </si>
+  <si>
+    <t>2. Hiển thị giao diện thông tin nhà xuất bản với mã nhà xuất bản đã được tạo sẵn
+3. Hiển thị icon thất bại, với tiêu đề thông báo "Thông báo", nội dung: "Sửa thông tin nhà xuất bản không thành công"
+4. Tắt thông báo</t>
+  </si>
+  <si>
+    <t>PUBLISHER_F_13</t>
+  </si>
+  <si>
+    <t>Xóa thông tin nhà xuất bản thành công</t>
+  </si>
+  <si>
+    <t>B1: Tại giao diện trang chủ, chọn nút nhà xuất bản hoặc chọn mục nhà xuất bản trong menu
+B2: Trong danh sách thông tin nhà xuất bản, chọn vào thông tin đầu tiên
+B3: Chọn nút xóa
+B4: Chọn nút "OK" trong thông báo</t>
+  </si>
+  <si>
+    <t>2. Hiển thị thông tin nhà xuất bản được chọn trên các trường tương ứng
+3. Hiển thị icon thông báo, với tiêu đề thông báo "Thông báo", nội dung: "Bạn có chắc chắn muốn xóa thông tin này không"
+4. Tắt thông báo và trở lại danh sách thông tin nhà xuất bản</t>
+  </si>
+  <si>
+    <t>PUBLISHER_F_14</t>
+  </si>
+  <si>
+    <t>Không xóa thông tin nhà xuất bản</t>
+  </si>
+  <si>
+    <t>B1: Tại giao diện trang chủ, chọn nút nhà xuất bản hoặc chọn mục nhà xuất bản trong menu
+B2: Trong danh sách thông tin nhà xuất bản, chọn vào thông tin đầu tiên
+B3: Chọn nút xóa
+B4: Chọn nút "CANCEL" trong thông báo</t>
+  </si>
+  <si>
+    <t>2. Hiển thị thông tin nhà xuất bản được chọn trên các trường tương ứng
+3. Hiển thị icon thông báo, với tiêu đề thông báo "Thông báo", nội dung: "Bạn có chắc chắn muốn xóa thông tin này không"
+4. Tắt thông báo</t>
+  </si>
+  <si>
+    <t>PUBLISHER_F_15</t>
+  </si>
+  <si>
+    <t>Xóa thông tin nhà xuất bản không tồn tại</t>
+  </si>
+  <si>
+    <t>B1: Tại giao diện trang chủ, chọn nút nhà xuất bản hoặc chọn mục nhà xuất bản trong menu
+B2: Chọn nút "+" để mở giao diện thông tin nhà xuất bản
+B3: Chọn nút xóa
+B4: Chọn nút "OK" trong thông báo
+B5: Chọn nút "OK" trong thông báo</t>
+  </si>
+  <si>
+    <t>2. Hiển thị thông tin nhà xuất bản được chọn trên các trường tương ứng
+3. Hiển thị icon thông báo, với tiêu đề thông báo "Thông báo", nội dung: "Bạn có chắc chắn muốn xóa thông tin này không"
+4. Hiển thị icon thông báo, với tiêu đề thông báo "Thông báo", nội dung: "Xóa thông tin nhà xuất bản không thành công"</t>
+  </si>
+  <si>
+    <t>PUBLISHER_F_16</t>
+  </si>
+  <si>
+    <t>Tìm kiếm thông tin nhà xuất bản với tên nhà xuất bản tồn tại</t>
+  </si>
+  <si>
+    <t>Đã đăng nhập thành công
+Có ít nhất một thông tin nhà xuất bản đã được lưu trong danh sách với tên 'kd'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1: Tại giao diện trang chủ, chọn nút nhà xuất bản hoặc chọn mục nhà xuất bản trong menu
+B2: Chọn nút tìm kiếm
+B3: Chọn ô tìm kiếm và nhập: 'kd'
+</t>
+  </si>
+  <si>
+    <t>3. Hiển thị thông tin các nhà xuất bản có tên 'kd'</t>
+  </si>
+  <si>
+    <t>PUBLISHER_F_17</t>
+  </si>
+  <si>
+    <t>Tìm kiếm thông tin nhà xuất bản với tên nhà xuất bản bị bỏ trống</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1: Tại giao diện trang chủ, chọn nút nhà xuất bản hoặc chọn mục nhà xuất bản trong menu
+B2: Chọn nút tìm kiếm
+B3: Chọn ô tìm kiếm và nhập: 'kd'
+B4: Xóa thông tin trong ô tìm kiếm
+</t>
+  </si>
+  <si>
+    <t>3. Hiển thị thông tin các nhà xuất bản có tên 'kd'
+4. Hiển thị toàn bộ thông tin các nhà xuất bản đã được lưu trữ</t>
+  </si>
+  <si>
+    <t>PUBLISHER_F_18</t>
+  </si>
+  <si>
+    <t>Tìm kiếm thông tin nhà xuất bản với tên nhà xuất bản không tồn tại</t>
+  </si>
+  <si>
+    <t>Đã đăng nhập thành công
+Có ít nhất một thông tin nhà xuất bản đã được lưu trong danh sách và không có nhà xuất bản nào có tên "kd"</t>
+  </si>
+  <si>
+    <t>3. Không hiển thị thông tin nhà xuất bản nào trong danh sách</t>
+  </si>
+  <si>
+    <t>Quản lý thông tin nhà xuất bản</t>
   </si>
 </sst>
 </file>
@@ -1358,7 +1343,47 @@
     <cellStyle name="Normal 2" xfId="3"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="46">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -1578,206 +1603,6 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -1856,14 +1681,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="C3:H11" totalsRowShown="0">
   <autoFilter ref="C3:H11"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Chức năng" dataDxfId="25"/>
-    <tableColumn id="2" name="Tổng số testcase" dataDxfId="24">
+    <tableColumn id="1" name="Chức năng" dataDxfId="29"/>
+    <tableColumn id="2" name="Tổng số testcase" dataDxfId="28">
       <calculatedColumnFormula>SUM(COUNTA('[1]Đăng nhập'!C12:C24), COUNTA('[1]Đăng kí'!C12:C26),COUNTA('[1]Khôi phục mật khẩu'!C12:C29))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Passed" dataDxfId="23"/>
-    <tableColumn id="4" name="Failed" dataDxfId="22"/>
-    <tableColumn id="5" name="N/A" dataDxfId="21"/>
-    <tableColumn id="6" name="Untested" dataDxfId="20"/>
+    <tableColumn id="3" name="Passed" dataDxfId="27"/>
+    <tableColumn id="4" name="Failed" dataDxfId="26"/>
+    <tableColumn id="5" name="N/A" dataDxfId="25"/>
+    <tableColumn id="6" name="Untested" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3343,7 +3168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D25" workbookViewId="0">
       <selection activeCell="G10" sqref="G10:I26"/>
     </sheetView>
   </sheetViews>
@@ -3458,410 +3283,410 @@
     </row>
     <row r="10" spans="2:9" ht="171.6" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
-        <v>130</v>
+        <v>171</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>131</v>
+        <v>172</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>132</v>
+        <v>173</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>133</v>
+        <v>174</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>134</v>
+        <v>175</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="11" t="s">
         <v>4</v>
       </c>
       <c r="I10" s="12">
-        <v>45370</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="171.6" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
-        <v>135</v>
+        <v>176</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>136</v>
+        <v>177</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>132</v>
+        <v>173</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>137</v>
+        <v>178</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>134</v>
+        <v>179</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="11" t="s">
         <v>4</v>
       </c>
       <c r="I11" s="12">
-        <v>45370</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" ht="171.6" x14ac:dyDescent="0.3">
+        <v>45369</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="196.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
-        <v>138</v>
+        <v>180</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>139</v>
+        <v>181</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>132</v>
+        <v>173</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>140</v>
+        <v>182</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>141</v>
+        <v>183</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="11" t="s">
         <v>4</v>
       </c>
       <c r="I12" s="12">
-        <v>45370</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" ht="171.6" x14ac:dyDescent="0.3">
+        <v>45369</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="132" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
-        <v>142</v>
+        <v>184</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>143</v>
+        <v>185</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>144</v>
+        <v>173</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>146</v>
+        <v>187</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="11" t="s">
         <v>4</v>
       </c>
       <c r="I13" s="12">
-        <v>45370</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="132" x14ac:dyDescent="0.3">
       <c r="B14" s="10" t="s">
-        <v>147</v>
+        <v>188</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>148</v>
+        <v>189</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>144</v>
+        <v>173</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>149</v>
+        <v>190</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>150</v>
+        <v>191</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="11" t="s">
         <v>4</v>
       </c>
       <c r="I14" s="12">
-        <v>45370</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" ht="132" x14ac:dyDescent="0.3">
+        <v>45369</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="118.8" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>152</v>
+        <v>193</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>153</v>
+        <v>194</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>154</v>
+        <v>195</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>155</v>
+        <v>196</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="11" t="s">
         <v>4</v>
       </c>
       <c r="I15" s="12">
-        <v>45370</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" ht="118.8" x14ac:dyDescent="0.3">
+        <v>45369</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="s">
-        <v>156</v>
+        <v>197</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>157</v>
+        <v>198</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>158</v>
+        <v>194</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>159</v>
+        <v>199</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="11" t="s">
         <v>4</v>
       </c>
       <c r="I16" s="12">
-        <v>45370</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
-        <v>161</v>
+        <v>201</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>162</v>
+        <v>202</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>163</v>
+        <v>194</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>164</v>
+        <v>203</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>165</v>
+        <v>204</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="11" t="s">
         <v>4</v>
       </c>
       <c r="I17" s="12">
-        <v>45370</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
+        <v>45369</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="118.8" x14ac:dyDescent="0.3">
       <c r="B18" s="10" t="s">
-        <v>166</v>
+        <v>205</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>167</v>
+        <v>206</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>169</v>
+        <v>207</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>170</v>
+        <v>208</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="11" t="s">
         <v>4</v>
       </c>
       <c r="I18" s="12">
-        <v>45370</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="118.8" x14ac:dyDescent="0.3">
       <c r="B19" s="10" t="s">
-        <v>171</v>
+        <v>209</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>172</v>
+        <v>210</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>158</v>
+        <v>194</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>173</v>
+        <v>211</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="G19" s="10"/>
       <c r="H19" s="11" t="s">
         <v>4</v>
       </c>
       <c r="I19" s="12">
-        <v>45370</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="132" x14ac:dyDescent="0.3">
       <c r="B20" s="10" t="s">
-        <v>175</v>
+        <v>213</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>176</v>
+        <v>214</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>158</v>
+        <v>194</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>177</v>
+        <v>215</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>178</v>
+        <v>216</v>
       </c>
       <c r="G20" s="10"/>
       <c r="H20" s="11" t="s">
         <v>4</v>
       </c>
       <c r="I20" s="12">
-        <v>45370</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="B21" s="10" t="s">
-        <v>179</v>
+        <v>217</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>180</v>
+        <v>218</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>158</v>
+        <v>194</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>181</v>
+        <v>219</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>182</v>
+        <v>220</v>
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="11" t="s">
         <v>4</v>
       </c>
       <c r="I21" s="12">
-        <v>45370</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="132" x14ac:dyDescent="0.3">
       <c r="B22" s="10" t="s">
-        <v>183</v>
+        <v>221</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>184</v>
+        <v>222</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>158</v>
+        <v>194</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>185</v>
+        <v>223</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>186</v>
+        <v>224</v>
       </c>
       <c r="G22" s="10"/>
       <c r="H22" s="11" t="s">
         <v>4</v>
       </c>
       <c r="I22" s="12">
-        <v>45370</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" ht="184.8" x14ac:dyDescent="0.3">
+        <v>45369</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="198" x14ac:dyDescent="0.3">
       <c r="B23" s="10" t="s">
-        <v>187</v>
+        <v>225</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>188</v>
+        <v>226</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>158</v>
+        <v>194</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>189</v>
+        <v>227</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>190</v>
+        <v>228</v>
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="11" t="s">
         <v>4</v>
       </c>
       <c r="I23" s="12">
-        <v>45370</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="92.4" x14ac:dyDescent="0.3">
       <c r="B24" s="10" t="s">
-        <v>191</v>
+        <v>229</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>192</v>
+        <v>230</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>193</v>
+        <v>231</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>194</v>
+        <v>232</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>195</v>
+        <v>233</v>
       </c>
       <c r="G24" s="10"/>
       <c r="H24" s="11" t="s">
         <v>4</v>
       </c>
       <c r="I24" s="12">
-        <v>45370</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="92.4" x14ac:dyDescent="0.3">
       <c r="B25" s="10" t="s">
-        <v>196</v>
+        <v>234</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>197</v>
+        <v>235</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>193</v>
+        <v>231</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>198</v>
+        <v>236</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>199</v>
+        <v>237</v>
       </c>
       <c r="G25" s="10"/>
       <c r="H25" s="11" t="s">
         <v>4</v>
       </c>
       <c r="I25" s="12">
-        <v>45370</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="105.6" x14ac:dyDescent="0.3">
       <c r="B26" s="10" t="s">
-        <v>200</v>
+        <v>238</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>201</v>
+        <v>239</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>202</v>
+        <v>240</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>194</v>
+        <v>232</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>203</v>
+        <v>241</v>
       </c>
       <c r="G26" s="10"/>
       <c r="H26" s="11" t="s">
         <v>4</v>
       </c>
       <c r="I26" s="12">
-        <v>45370</v>
+        <v>45369</v>
       </c>
     </row>
   </sheetData>
@@ -3894,7 +3719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -4009,19 +3834,19 @@
     </row>
     <row r="10" spans="2:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
-        <v>204</v>
+        <v>130</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>205</v>
+        <v>131</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>206</v>
+        <v>132</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>207</v>
+        <v>133</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>208</v>
+        <v>134</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="11" t="s">
@@ -4033,19 +3858,19 @@
     </row>
     <row r="11" spans="2:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
-        <v>209</v>
+        <v>135</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>210</v>
+        <v>136</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>206</v>
+        <v>132</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>211</v>
+        <v>137</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>208</v>
+        <v>134</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="11" t="s">
@@ -4057,19 +3882,19 @@
     </row>
     <row r="12" spans="2:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
-        <v>212</v>
+        <v>138</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>213</v>
+        <v>139</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>206</v>
+        <v>132</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>214</v>
+        <v>140</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>215</v>
+        <v>141</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="11" t="s">
@@ -4081,19 +3906,19 @@
     </row>
     <row r="13" spans="2:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
-        <v>216</v>
+        <v>142</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>217</v>
+        <v>143</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>206</v>
+        <v>132</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>218</v>
+        <v>144</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>215</v>
+        <v>141</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="11" t="s">
@@ -4105,19 +3930,19 @@
     </row>
     <row r="14" spans="2:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="B14" s="10" t="s">
-        <v>219</v>
+        <v>145</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>220</v>
+        <v>146</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>206</v>
+        <v>132</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>221</v>
+        <v>147</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>215</v>
+        <v>141</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="11" t="s">
@@ -4129,19 +3954,19 @@
     </row>
     <row r="15" spans="2:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
-        <v>222</v>
+        <v>148</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>223</v>
+        <v>149</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>206</v>
+        <v>132</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>224</v>
+        <v>150</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>225</v>
+        <v>151</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="11" t="s">
@@ -4153,19 +3978,19 @@
     </row>
     <row r="16" spans="2:9" ht="250.8" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="s">
-        <v>226</v>
+        <v>152</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>227</v>
+        <v>153</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>206</v>
+        <v>132</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>228</v>
+        <v>154</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>229</v>
+        <v>155</v>
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="11" t="s">
@@ -4177,19 +4002,19 @@
     </row>
     <row r="17" spans="2:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
-        <v>230</v>
+        <v>156</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>231</v>
+        <v>157</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>206</v>
+        <v>132</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>232</v>
+        <v>158</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>233</v>
+        <v>159</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="11" t="s">
@@ -4229,8 +4054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4242,16 +4067,16 @@
   <sheetData>
     <row r="3" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>234</v>
+        <v>160</v>
       </c>
       <c r="D3" t="s">
-        <v>235</v>
+        <v>161</v>
       </c>
       <c r="E3" t="s">
-        <v>236</v>
+        <v>162</v>
       </c>
       <c r="F3" t="s">
-        <v>237</v>
+        <v>163</v>
       </c>
       <c r="G3" t="s">
         <v>3</v>
@@ -4262,7 +4087,7 @@
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C4" s="14" t="s">
-        <v>238</v>
+        <v>164</v>
       </c>
       <c r="D4" s="15">
         <f>SUM(Table2[[#This Row],[Passed]:[Untested]])</f>
@@ -4287,7 +4112,7 @@
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C5" s="14" t="s">
-        <v>239</v>
+        <v>165</v>
       </c>
       <c r="D5" s="15">
         <f>SUM(Table2[[#This Row],[Passed]:[Untested]])</f>
@@ -4312,7 +4137,7 @@
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C6" s="14" t="s">
-        <v>240</v>
+        <v>166</v>
       </c>
       <c r="D6" s="15">
         <f>SUM(Table2[[#This Row],[Passed]:[Untested]])</f>
@@ -4337,32 +4162,32 @@
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C7" s="14" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D7" s="15">
         <f>SUM(Table2[[#This Row],[Passed]:[Untested]])</f>
         <v>17</v>
       </c>
       <c r="E7" s="15">
-        <f>COLLECTION!F4</f>
+        <f>PUBLISHER!F4</f>
         <v>0</v>
       </c>
       <c r="F7" s="15">
-        <f>COLLECTION!G4</f>
+        <f>PUBLISHER!G4</f>
         <v>0</v>
       </c>
       <c r="G7" s="15">
-        <f>COLLECTION!H4</f>
+        <f>PUBLISHER!H4</f>
         <v>0</v>
       </c>
       <c r="H7" s="15">
-        <f>COLLECTION!I4</f>
+        <f>PUBLISHER!I4</f>
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C8" s="14" t="s">
-        <v>242</v>
+        <v>167</v>
       </c>
       <c r="D8" s="15">
         <f>SUM(Table2[[#This Row],[Passed]:[Untested]])</f>
@@ -4387,7 +4212,7 @@
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C9" s="18" t="s">
-        <v>243</v>
+        <v>168</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
@@ -4397,7 +4222,7 @@
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C10" s="14" t="s">
-        <v>244</v>
+        <v>169</v>
       </c>
       <c r="D10" s="16">
         <f>SUM(D4:D8)</f>
@@ -4422,7 +4247,7 @@
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C11" s="14" t="s">
-        <v>245</v>
+        <v>170</v>
       </c>
       <c r="D11" s="20">
         <v>1</v>

</xml_diff>

<commit_message>
fix some issues in TC
</commit_message>
<xml_diff>
--- a/Auto_TC.xlsx
+++ b/Auto_TC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="108" windowWidth="14808" windowHeight="6984" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="6984" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LOGIN" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="245">
   <si>
     <t>TEST CASES</t>
   </si>
@@ -591,10 +591,6 @@
   <si>
     <t>Đã cài đặt ứng dụng thành công
 Chưa có tài khoản đăng kí trong hệ thống</t>
-  </si>
-  <si>
-    <t>7. Hiển thị icon cảnh báo, với tiêu đề thông báo "cảnh báo", nội dung: "Chưa có tài khoản đăng kí trong hệ thống"
-8. Tắt thông báo</t>
   </si>
   <si>
     <t>SETUP_ACCOUNT_F_00</t>
@@ -1127,6 +1123,19 @@
 B10: Chọn ảnh bất kì trong thư viện
 B11: Chọn nút "Lưu"
 B12: Nhấn nút "OK" trong thông báo</t>
+  </si>
+  <si>
+    <t>B1: Mở ứng dụng
+B2: Chọn "Quên mật khẩu"
+B3: Nhấn chọn trường tên đăng nhập và nhập: 'hi'
+B4: Nhấn chọn trường mật khẩu và nhập: '12'
+B5: Nhấn chọn trường xác nhận mật khẩu và nhập: '12'
+B6: Chọn gửi mã xác nhận
+B7: Chọn nút "OK" trên thông báo</t>
+  </si>
+  <si>
+    <t>6. Hiển thị icon thông báo, với tiêu đề thông báo "Thông báo", nội dung: "Chưa có tài khoản đăng kí trong hệ thống do chưa đăng kí tài khoản"
+7. Tắt thông báo</t>
   </si>
 </sst>
 </file>
@@ -2712,8 +2721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="F19" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10:G21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3083,7 +3092,7 @@
         <v>45368</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" ht="92.4" x14ac:dyDescent="0.3">
       <c r="B21" s="10" t="s">
         <v>126</v>
       </c>
@@ -3094,10 +3103,10 @@
         <v>128</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>91</v>
+        <v>243</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>129</v>
+        <v>244</v>
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="11" t="s">
@@ -3252,19 +3261,19 @@
     </row>
     <row r="10" spans="2:9" ht="171.6" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>173</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>174</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="11" t="s">
@@ -3276,19 +3285,19 @@
     </row>
     <row r="11" spans="2:9" ht="171.6" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="D11" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="E11" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>177</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>178</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="11" t="s">
@@ -3300,19 +3309,19 @@
     </row>
     <row r="12" spans="2:9" ht="196.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>181</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>182</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="11" t="s">
@@ -3324,19 +3333,19 @@
     </row>
     <row r="13" spans="2:9" ht="132" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="D13" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="E13" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>185</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>186</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="11" t="s">
@@ -3348,19 +3357,19 @@
     </row>
     <row r="14" spans="2:9" ht="132" x14ac:dyDescent="0.3">
       <c r="B14" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="D14" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="F14" s="10" t="s">
         <v>188</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>189</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="11" t="s">
@@ -3372,19 +3381,19 @@
     </row>
     <row r="15" spans="2:9" ht="118.8" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="D15" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="E15" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>193</v>
-      </c>
       <c r="F15" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="11" t="s">
@@ -3396,19 +3405,19 @@
     </row>
     <row r="16" spans="2:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="D16" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="E16" s="10" t="s">
+      <c r="F16" s="10" t="s">
         <v>196</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>197</v>
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="11" t="s">
@@ -3420,19 +3429,19 @@
     </row>
     <row r="17" spans="2:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="F17" s="10" t="s">
         <v>198</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>199</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="11" t="s">
@@ -3444,19 +3453,19 @@
     </row>
     <row r="18" spans="2:9" ht="118.8" x14ac:dyDescent="0.3">
       <c r="B18" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="D18" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="F18" s="10" t="s">
         <v>201</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>202</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="11" t="s">
@@ -3468,19 +3477,19 @@
     </row>
     <row r="19" spans="2:9" ht="118.8" x14ac:dyDescent="0.3">
       <c r="B19" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="D19" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="D19" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="E19" s="10" t="s">
+      <c r="F19" s="10" t="s">
         <v>205</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>206</v>
       </c>
       <c r="G19" s="10"/>
       <c r="H19" s="11" t="s">
@@ -3492,19 +3501,19 @@
     </row>
     <row r="20" spans="2:9" ht="132" x14ac:dyDescent="0.3">
       <c r="B20" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="D20" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="E20" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="D20" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>209</v>
-      </c>
       <c r="F20" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G20" s="10"/>
       <c r="H20" s="11" t="s">
@@ -3516,19 +3525,19 @@
     </row>
     <row r="21" spans="2:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="B21" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="D21" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F21" s="10" t="s">
         <v>211</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>212</v>
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="11" t="s">
@@ -3540,19 +3549,19 @@
     </row>
     <row r="22" spans="2:9" ht="132" x14ac:dyDescent="0.3">
       <c r="B22" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="D22" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="E22" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="D22" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="E22" s="10" t="s">
+      <c r="F22" s="10" t="s">
         <v>215</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>216</v>
       </c>
       <c r="G22" s="10"/>
       <c r="H22" s="11" t="s">
@@ -3564,19 +3573,19 @@
     </row>
     <row r="23" spans="2:9" ht="184.8" x14ac:dyDescent="0.3">
       <c r="B23" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="D23" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="E23" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="D23" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>219</v>
-      </c>
       <c r="F23" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="11" t="s">
@@ -3588,19 +3597,19 @@
     </row>
     <row r="24" spans="2:9" ht="92.4" x14ac:dyDescent="0.3">
       <c r="B24" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="D24" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="E24" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="F24" s="10" t="s">
         <v>223</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>224</v>
       </c>
       <c r="G24" s="10"/>
       <c r="H24" s="11" t="s">
@@ -3612,19 +3621,19 @@
     </row>
     <row r="25" spans="2:9" ht="92.4" x14ac:dyDescent="0.3">
       <c r="B25" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="D25" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="E25" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="E25" s="10" t="s">
+      <c r="F25" s="10" t="s">
         <v>227</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>228</v>
       </c>
       <c r="G25" s="10"/>
       <c r="H25" s="11" t="s">
@@ -3636,19 +3645,19 @@
     </row>
     <row r="26" spans="2:9" ht="118.8" x14ac:dyDescent="0.3">
       <c r="B26" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="D26" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="F26" s="10" t="s">
         <v>230</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>231</v>
       </c>
       <c r="G26" s="10"/>
       <c r="H26" s="11" t="s">
@@ -3688,7 +3697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -3803,19 +3812,19 @@
     </row>
     <row r="10" spans="2:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>133</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>134</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="11" t="s">
@@ -3827,19 +3836,19 @@
     </row>
     <row r="11" spans="2:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="D11" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>137</v>
-      </c>
       <c r="F11" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="11" t="s">
@@ -3851,19 +3860,19 @@
     </row>
     <row r="12" spans="2:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>141</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="11" t="s">
@@ -3875,19 +3884,19 @@
     </row>
     <row r="13" spans="2:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="D13" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>144</v>
-      </c>
       <c r="F13" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="11" t="s">
@@ -3899,19 +3908,19 @@
     </row>
     <row r="14" spans="2:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="B14" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="D14" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>147</v>
-      </c>
       <c r="F14" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="11" t="s">
@@ -3923,19 +3932,19 @@
     </row>
     <row r="15" spans="2:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="D15" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="E15" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>150</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>151</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="11" t="s">
@@ -3947,19 +3956,19 @@
     </row>
     <row r="16" spans="2:9" ht="250.8" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="D16" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>153</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>154</v>
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="11" t="s">
@@ -3971,19 +3980,19 @@
     </row>
     <row r="17" spans="2:9" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="D17" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="E17" s="10" t="s">
+      <c r="F17" s="10" t="s">
         <v>157</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>158</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="11" t="s">
@@ -4036,16 +4045,16 @@
   <sheetData>
     <row r="3" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" t="s">
         <v>159</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>160</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>161</v>
-      </c>
-      <c r="F3" t="s">
-        <v>162</v>
       </c>
       <c r="G3" t="s">
         <v>3</v>
@@ -4056,7 +4065,7 @@
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C4" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D4" s="15">
         <f>SUM(Table2[[#This Row],[Passed]:[Untested]])</f>
@@ -4081,7 +4090,7 @@
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C5" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D5" s="15">
         <f>SUM(Table2[[#This Row],[Passed]:[Untested]])</f>
@@ -4106,7 +4115,7 @@
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C6" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D6" s="15">
         <f>SUM(Table2[[#This Row],[Passed]:[Untested]])</f>
@@ -4131,7 +4140,7 @@
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C7" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D7" s="15">
         <f>SUM(Table2[[#This Row],[Passed]:[Untested]])</f>
@@ -4156,7 +4165,7 @@
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C8" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D8" s="15">
         <f>SUM(Table2[[#This Row],[Passed]:[Untested]])</f>
@@ -4181,7 +4190,7 @@
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C9" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
@@ -4191,7 +4200,7 @@
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C10" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D10" s="16">
         <f>SUM(D4:D8)</f>
@@ -4216,7 +4225,7 @@
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C11" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D11" s="20">
         <v>1</v>

</xml_diff>